<commit_message>
Edited template to include a field for addresses
</commit_message>
<xml_diff>
--- a/dnac/data_sources/LSDD-Form-SDA-optimized-full.xlsx
+++ b/dnac/data_sources/LSDD-Form-SDA-optimized-full.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="137">
   <si>
     <t>Network Hierarchy</t>
   </si>
@@ -418,6 +418,21 @@
   </si>
   <si>
     <t>Building</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Leicester</t>
   </si>
 </sst>
 </file>
@@ -1087,8 +1102,8 @@
       <sheetName val="Backups"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="19">
           <cell r="B19" t="str">
@@ -1106,20 +1121,20 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1415,14 +1430,14 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1461,7 +1476,9 @@
       <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="7" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -1476,7 +1493,9 @@
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
@@ -1491,7 +1510,9 @@
       <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
@@ -1504,7 +1525,9 @@
       <c r="D7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
@@ -1517,7 +1540,9 @@
       <c r="D8" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -1532,7 +1557,9 @@
       <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
@@ -1547,7 +1574,9 @@
       <c r="D10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1560,7 +1589,9 @@
       <c r="D11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1573,7 +1604,9 @@
       <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -1981,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed duplicate addition and deletion issue + refactored the checkTaskExecutionStatus in order to work for both addition and deletion functions.
</commit_message>
<xml_diff>
--- a/dnac/data_sources/LSDD-Form-SDA-optimized-full.xlsx
+++ b/dnac/data_sources/LSDD-Form-SDA-optimized-full.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="140">
   <si>
     <t>Network Hierarchy</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1438,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
Save new version of SDA data capture working file
</commit_message>
<xml_diff>
--- a/dnac/data_sources/LSDD-Form-SDA-optimized-full.xlsx
+++ b/dnac/data_sources/LSDD-Form-SDA-optimized-full.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NetHie" sheetId="1" r:id="rId1"/>
-    <sheet name="VRFs&amp;VNs" sheetId="2" r:id="rId2"/>
-    <sheet name="NetSrv" sheetId="3" r:id="rId3"/>
+    <sheet name="VRFs" sheetId="4" r:id="rId2"/>
+    <sheet name="VNs" sheetId="2" r:id="rId3"/>
+    <sheet name="NetSrv" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1437,7 +1438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -1643,10 +1644,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A3:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
+    </row>
+    <row r="4" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,110 +1820,200 @@
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
       <c r="J3" s="23"/>
     </row>
-    <row r="4" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="G4" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="H4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="I4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
       <c r="J4" s="23"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+    <row r="5" spans="1:10" ht="73.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="J5" s="23"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+    <row r="6" spans="1:10" ht="85.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="29"/>
       <c r="J6" s="23"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+    <row r="7" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="J7" s="23"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+    <row r="8" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="A9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="30"/>
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="A10" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1802,227 +2028,17 @@
       <c r="I11" s="22"/>
       <c r="J11" s="23"/>
     </row>
-    <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="1:10" ht="73.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10" ht="85.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2030,7 +2046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>

</xml_diff>